<commit_message>
Added line with number of elements (bags)
</commit_message>
<xml_diff>
--- a/ListMakerTwo/Templates/ReceiverSummeryTemplate01.xlsx
+++ b/ListMakerTwo/Templates/ReceiverSummeryTemplate01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Henrik\Dropbox\DevProjects\LugbulkListMaker\ListMakerTwo\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Dropbox\DevProjects\LugbulkListMaker\ListMakerTwo\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29055133-47FA-41FD-941D-2EAAA7DBE7FE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EB52FA-10E2-4160-AFD1-63DDB1F19080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="9870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2940" windowWidth="20475" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ElementId</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>X - Name</t>
+  </si>
+  <si>
+    <t>Number of bags</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -123,11 +126,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -143,16 +157,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,50 +499,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-    </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -797,11 +819,18 @@
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>